<commit_message>
Reduced scale of Q23
</commit_message>
<xml_diff>
--- a/Discriptive tables.xlsx
+++ b/Discriptive tables.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="66">
   <si>
     <t>38. Насколько приемлемой большинство Ваших коллег в подразделении сочтет следующую деятельность (позицию)? Полицейский является ярым противником подработок полицейских</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>Sig</t>
+  </si>
+  <si>
+    <t>Слабая положительная связь</t>
+  </si>
+  <si>
+    <t>Частота</t>
+  </si>
+  <si>
+    <t>% ответивших</t>
   </si>
 </sst>
 </file>
@@ -268,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -311,8 +320,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -376,8 +424,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -399,14 +515,29 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="131">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -438,6 +569,40 @@
     <cellStyle name="Гиперссылка" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -470,6 +635,40 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="130" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -4095,10 +4294,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4110,37 +4309,60 @@
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="19" max="19" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="E4" s="9" t="s">
+    <row r="4" spans="1:37">
+      <c r="E4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="L4" s="9" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="L4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="S4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AC4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+    </row>
+    <row r="5" spans="1:37">
       <c r="A5" s="6"/>
       <c r="B5" s="8">
         <v>39</v>
@@ -4176,8 +4398,24 @@
       <c r="Q5" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="AD5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK5" s="14"/>
+    </row>
+    <row r="6" spans="1:37">
       <c r="A6" s="6" t="s">
         <v>44</v>
       </c>
@@ -4223,8 +4461,49 @@
       <c r="Q6" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="S6" s="1"/>
+      <c r="T6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="U6" s="12"/>
+      <c r="V6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6" s="14"/>
+      <c r="X6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA6" s="14"/>
+      <c r="AD6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK6" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
       <c r="A7" s="6" t="s">
         <v>45</v>
       </c>
@@ -4266,8 +4545,56 @@
       <c r="Q7" s="1">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="S7" s="1"/>
+      <c r="T7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+    </row>
+    <row r="8" spans="1:37">
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
         <v>52</v>
@@ -4300,8 +4627,54 @@
       <c r="Q8" s="1">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="S8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="1">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="V8" s="1">
+        <v>26</v>
+      </c>
+      <c r="W8" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="X8" s="1">
+        <v>68</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>11</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+    </row>
+    <row r="9" spans="1:37">
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
         <v>51</v>
@@ -4334,8 +4707,62 @@
       <c r="Q9" s="1">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="S9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" s="1">
+        <v>75</v>
+      </c>
+      <c r="U9" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="V9" s="1">
+        <v>46</v>
+      </c>
+      <c r="W9" s="1">
+        <v>12</v>
+      </c>
+      <c r="X9" s="1">
+        <v>108</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>29.1</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>19</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>4</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
         <v>50</v>
@@ -4368,8 +4795,62 @@
       <c r="Q10" s="1">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="S10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T10" s="1">
+        <v>65</v>
+      </c>
+      <c r="U10" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="V10" s="1">
+        <v>45</v>
+      </c>
+      <c r="W10" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="X10" s="1">
+        <v>37</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>8</v>
+      </c>
+      <c r="AG10" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="2">
+        <v>17</v>
+      </c>
+      <c r="AI10" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AJ10" s="2">
+        <v>11</v>
+      </c>
+      <c r="AK10" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37">
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -4400,8 +4881,62 @@
       <c r="Q11" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="S11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="T11" s="1">
+        <v>152</v>
+      </c>
+      <c r="U11" s="1">
+        <v>40.1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>167</v>
+      </c>
+      <c r="W11" s="1">
+        <v>43.7</v>
+      </c>
+      <c r="X11" s="1">
+        <v>69</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>178</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>38</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="2">
+        <v>12</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>29</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>7</v>
+      </c>
+      <c r="AJ11" s="2">
+        <v>13</v>
+      </c>
+      <c r="AK11" s="2">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
       <c r="E12" s="2" t="s">
         <v>45</v>
       </c>
@@ -4432,8 +4967,62 @@
       <c r="Q12" s="1">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="S12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T12" s="1">
+        <v>61</v>
+      </c>
+      <c r="U12" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="V12" s="1">
+        <v>98</v>
+      </c>
+      <c r="W12" s="1">
+        <v>25.7</v>
+      </c>
+      <c r="X12" s="1">
+        <v>89</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>237</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>50.6</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="2">
+        <v>56</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>12.9</v>
+      </c>
+      <c r="AF12" s="2">
+        <v>54</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>13.4</v>
+      </c>
+      <c r="AH12" s="2">
+        <v>74</v>
+      </c>
+      <c r="AI12" s="2">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="AJ12" s="2">
+        <v>43</v>
+      </c>
+      <c r="AK12" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
       <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
@@ -4462,8 +5051,35 @@
       <c r="Q13" s="1">
         <v>39.799999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="AC13" s="2">
+        <v>6</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>25</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>30</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>7.3</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>17</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
       <c r="L14" s="1"/>
       <c r="M14" s="1">
         <v>8</v>
@@ -4480,8 +5096,35 @@
       <c r="Q14" s="1">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="AC14" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD14" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="AF14" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="AH14" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="AJ14" s="2">
+        <v>46</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
       <c r="L15" s="1"/>
       <c r="M15" s="1">
         <v>9</v>
@@ -4498,8 +5141,35 @@
       <c r="Q15" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="AC15" s="2">
+        <v>8</v>
+      </c>
+      <c r="AD15" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE15" s="2">
+        <v>17</v>
+      </c>
+      <c r="AF15" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG15" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AH15" s="2">
+        <v>46</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="AJ15" s="2">
+        <v>72</v>
+      </c>
+      <c r="AK15" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
       <c r="E16">
         <v>1</v>
       </c>
@@ -4522,8 +5192,35 @@
       <c r="Q16" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="5:17">
+      <c r="AC16" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>7.8</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>37</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>34</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AJ16" s="2">
+        <v>68</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="17" spans="5:37">
       <c r="E17">
         <v>2</v>
       </c>
@@ -4544,8 +5241,35 @@
         <v>100</v>
       </c>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="5:17">
+      <c r="AC17" s="2">
+        <v>10</v>
+      </c>
+      <c r="AD17" s="2">
+        <v>132</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="AF17" s="2">
+        <v>175</v>
+      </c>
+      <c r="AG17" s="2">
+        <v>43.3</v>
+      </c>
+      <c r="AH17" s="2">
+        <v>125</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="AJ17" s="2">
+        <v>209</v>
+      </c>
+      <c r="AK17" s="2">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:37">
       <c r="E18">
         <v>3</v>
       </c>
@@ -4567,7 +5291,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="5:17">
+    <row r="19" spans="5:37">
       <c r="E19">
         <v>4</v>
       </c>
@@ -4587,7 +5311,7 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="5:17">
+    <row r="20" spans="5:37">
       <c r="E20">
         <v>5</v>
       </c>
@@ -4595,7 +5319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="5:17">
+    <row r="22" spans="5:37">
       <c r="M22">
         <v>0</v>
       </c>
@@ -4603,53 +5327,53 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="5:17">
+    <row r="23" spans="5:37">
       <c r="M23" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="5:17">
+    <row r="24" spans="5:37">
       <c r="M24" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="5:17">
+    <row r="25" spans="5:37">
       <c r="M25" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="5:17">
+    <row r="26" spans="5:37">
       <c r="M26" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="5:17">
+    <row r="27" spans="5:37">
       <c r="M27" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="5:17">
+    <row r="28" spans="5:37">
       <c r="M28" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="5:17">
+    <row r="29" spans="5:37">
       <c r="M29" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="5:17">
+    <row r="30" spans="5:37">
       <c r="M30" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="5:17">
+    <row r="31" spans="5:37">
       <c r="M31" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="5:17">
-      <c r="M32" s="10">
+    <row r="32" spans="5:37">
+      <c r="M32" s="11">
         <v>10</v>
       </c>
       <c r="N32" s="1" t="s">
@@ -4657,9 +5381,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="12">
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AC4:AK4"/>
     <mergeCell ref="L4:Q4"/>
     <mergeCell ref="E4:J4"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="S4:AA4"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4673,23 +5407,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:F4"/>
+  <dimension ref="E1:H4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="5:6">
+    <row r="1" spans="5:8">
       <c r="E1" t="s">
         <v>60</v>
       </c>
       <c r="F1">
         <v>0.16800000000000001</v>
       </c>
-    </row>
-    <row r="2" spans="5:6">
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="5:8">
       <c r="E2" t="s">
         <v>62</v>
       </c>
@@ -4697,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="5:6">
+    <row r="3" spans="5:8">
       <c r="E3" t="s">
         <v>61</v>
       </c>
@@ -4705,7 +5442,7 @@
         <v>0.20599999999999999</v>
       </c>
     </row>
-    <row r="4" spans="5:6">
+    <row r="4" spans="5:8">
       <c r="E4" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Final of Apr 10
</commit_message>
<xml_diff>
--- a/Discriptive tables.xlsx
+++ b/Discriptive tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="модель с 3 индикаторами" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="73">
   <si>
     <t>38. Насколько приемлемой большинство Ваших коллег в подразделении сочтет следующую деятельность (позицию)? Полицейский является ярым противником подработок полицейских</t>
   </si>
@@ -213,20 +213,41 @@
     <t>Sig</t>
   </si>
   <si>
-    <t>Слабая положительная связь</t>
+    <t>Страна</t>
   </si>
   <si>
     <t>Частота</t>
   </si>
   <si>
     <t>% ответивших</t>
+  </si>
+  <si>
+    <t>В некоторых странах полиция и другие официальные органы согласны идти навстречу тем, кто нарушает правила, и люди могут</t>
+  </si>
+  <si>
+    <t>,140**</t>
+  </si>
+  <si>
+    <t>,164**</t>
+  </si>
+  <si>
+    <t>,192**</t>
+  </si>
+  <si>
+    <t>,222**</t>
+  </si>
+  <si>
+    <t>,089*</t>
+  </si>
+  <si>
+    <t>,097*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -262,8 +283,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +302,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +395,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -492,8 +527,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -536,8 +667,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="227">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -603,6 +744,54 @@
     <cellStyle name="Гиперссылка" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -669,6 +858,54 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="226" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1000,7 +1237,7 @@
   <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2433,11 +2670,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="O37" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="17" max="17" width="178.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -3347,7 +3587,7 @@
       <c r="R42" s="4">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="S42" s="5">
+      <c r="S42" s="19">
         <v>0.39400000000000002</v>
       </c>
       <c r="U42">
@@ -4294,10 +4534,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK32"/>
+  <dimension ref="A1:AV69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA28" sqref="AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4312,17 +4552,30 @@
     <col min="19" max="19" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:48">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:48">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="3" spans="1:48">
+      <c r="AN3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO3" s="9"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="9"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9"/>
+      <c r="AV3" s="9"/>
+    </row>
+    <row r="4" spans="1:48">
       <c r="E4" s="10" t="s">
         <v>58</v>
       </c>
@@ -4361,8 +4614,24 @@
       <c r="AI4" s="9"/>
       <c r="AJ4" s="9"/>
       <c r="AK4" s="9"/>
-    </row>
-    <row r="5" spans="1:37">
+      <c r="AN4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS4" s="14"/>
+      <c r="AT4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU4" s="14"/>
+    </row>
+    <row r="5" spans="1:48">
       <c r="A5" s="6"/>
       <c r="B5" s="8">
         <v>39</v>
@@ -4414,8 +4683,32 @@
         <v>32</v>
       </c>
       <c r="AK5" s="14"/>
-    </row>
-    <row r="6" spans="1:37">
+      <c r="AN5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AO5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU5" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48">
       <c r="A6" s="6" t="s">
         <v>44</v>
       </c>
@@ -4502,8 +4795,35 @@
       <c r="AK6" s="15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:37">
+      <c r="AM6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>4</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>4</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48">
       <c r="A7" s="6" t="s">
         <v>45</v>
       </c>
@@ -4593,8 +4913,35 @@
       </c>
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
-    </row>
-    <row r="8" spans="1:37">
+      <c r="AM7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>18</v>
+      </c>
+      <c r="AO7" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AP7" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="AQ7" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="AR7" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AS7" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="AT7" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="AU7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48">
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
         <v>52</v>
@@ -4673,8 +5020,35 @@
       </c>
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
-    </row>
-    <row r="9" spans="1:37">
+      <c r="AM8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>98</v>
+      </c>
+      <c r="AO8" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="AP8" s="2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AQ8" s="2">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="AR8" s="2">
+        <v>23</v>
+      </c>
+      <c r="AS8" s="2">
+        <v>25.2</v>
+      </c>
+      <c r="AT8" s="2">
+        <v>11.9</v>
+      </c>
+      <c r="AU8" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48">
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
         <v>51</v>
@@ -4761,8 +5135,35 @@
       <c r="AK9" s="2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:37">
+      <c r="AM9" s="2">
+        <v>4</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>149</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="AP9" s="2">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="AQ9" s="2">
+        <v>21.8</v>
+      </c>
+      <c r="AR9" s="2">
+        <v>19</v>
+      </c>
+      <c r="AS9" s="2">
+        <v>20.8</v>
+      </c>
+      <c r="AT9" s="2">
+        <v>23.4</v>
+      </c>
+      <c r="AU9" s="2">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48">
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
         <v>50</v>
@@ -4849,8 +5250,35 @@
       <c r="AK10" s="2">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:37">
+      <c r="AM10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN10" s="2">
+        <v>166</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="AP10" s="2">
+        <v>47.1</v>
+      </c>
+      <c r="AQ10" s="2">
+        <v>52.5</v>
+      </c>
+      <c r="AR10" s="2">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="AS10" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="AT10" s="2">
+        <v>55</v>
+      </c>
+      <c r="AU10" s="2">
+        <v>57.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48">
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -4936,7 +5364,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:48">
       <c r="E12" s="2" t="s">
         <v>45</v>
       </c>
@@ -5022,7 +5450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:48">
       <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
@@ -5079,7 +5507,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:48">
       <c r="L14" s="1"/>
       <c r="M14" s="1">
         <v>8</v>
@@ -5124,7 +5552,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:48">
       <c r="L15" s="1"/>
       <c r="M15" s="1">
         <v>9</v>
@@ -5169,7 +5597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:48">
       <c r="E16">
         <v>1</v>
       </c>
@@ -5380,13 +5808,560 @@
         <v>57</v>
       </c>
     </row>
+    <row r="36" spans="11:17">
+      <c r="K36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="11:17">
+      <c r="K37" t="s">
+        <v>63</v>
+      </c>
+      <c r="N37" t="s">
+        <v>46</v>
+      </c>
+      <c r="O37" t="s">
+        <v>47</v>
+      </c>
+      <c r="P37" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="11:17">
+      <c r="K38" t="s">
+        <v>6</v>
+      </c>
+      <c r="L38" t="s">
+        <v>44</v>
+      </c>
+      <c r="M38" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38">
+        <v>4</v>
+      </c>
+      <c r="O38">
+        <v>0.9</v>
+      </c>
+      <c r="P38">
+        <v>0.9</v>
+      </c>
+      <c r="Q38">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="39" spans="11:17">
+      <c r="M39">
+        <v>2</v>
+      </c>
+      <c r="N39">
+        <v>18</v>
+      </c>
+      <c r="O39">
+        <v>4</v>
+      </c>
+      <c r="P39">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q39">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="11:17">
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <v>98</v>
+      </c>
+      <c r="O40">
+        <v>21.9</v>
+      </c>
+      <c r="P40">
+        <v>22.5</v>
+      </c>
+      <c r="Q40">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="41" spans="11:17">
+      <c r="M41">
+        <v>4</v>
+      </c>
+      <c r="N41">
+        <v>149</v>
+      </c>
+      <c r="O41">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="P41">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="Q41">
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="42" spans="11:17">
+      <c r="M42" t="s">
+        <v>57</v>
+      </c>
+      <c r="N42">
+        <v>166</v>
+      </c>
+      <c r="O42">
+        <v>37.1</v>
+      </c>
+      <c r="P42">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="Q42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="11:17">
+      <c r="M43" t="s">
+        <v>19</v>
+      </c>
+      <c r="N43">
+        <v>435</v>
+      </c>
+      <c r="O43">
+        <v>97.1</v>
+      </c>
+      <c r="P43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="11:17">
+      <c r="L44" t="s">
+        <v>45</v>
+      </c>
+      <c r="M44" t="s">
+        <v>55</v>
+      </c>
+      <c r="N44">
+        <v>13</v>
+      </c>
+      <c r="O44">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="45" spans="11:17">
+      <c r="L45" t="s">
+        <v>19</v>
+      </c>
+      <c r="N45">
+        <v>448</v>
+      </c>
+      <c r="O45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="11:17">
+      <c r="K46" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46" t="s">
+        <v>44</v>
+      </c>
+      <c r="M46" t="s">
+        <v>56</v>
+      </c>
+      <c r="N46">
+        <v>10</v>
+      </c>
+      <c r="O46">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P46">
+        <v>2.5</v>
+      </c>
+      <c r="Q46">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="47" spans="11:17">
+      <c r="M47">
+        <v>2</v>
+      </c>
+      <c r="N47">
+        <v>15</v>
+      </c>
+      <c r="O47">
+        <v>3.3</v>
+      </c>
+      <c r="P47">
+        <v>3.7</v>
+      </c>
+      <c r="Q47">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="48" spans="11:17">
+      <c r="M48">
+        <v>3</v>
+      </c>
+      <c r="N48">
+        <v>79</v>
+      </c>
+      <c r="O48">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="P48">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="Q48">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="49" spans="11:17">
+      <c r="M49">
+        <v>4</v>
+      </c>
+      <c r="N49">
+        <v>88</v>
+      </c>
+      <c r="O49">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="P49">
+        <v>21.8</v>
+      </c>
+      <c r="Q49">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="50" spans="11:17">
+      <c r="M50" t="s">
+        <v>57</v>
+      </c>
+      <c r="N50">
+        <v>212</v>
+      </c>
+      <c r="O50">
+        <v>47.1</v>
+      </c>
+      <c r="P50">
+        <v>52.5</v>
+      </c>
+      <c r="Q50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="11:17">
+      <c r="M51" t="s">
+        <v>19</v>
+      </c>
+      <c r="N51">
+        <v>404</v>
+      </c>
+      <c r="O51">
+        <v>89.8</v>
+      </c>
+      <c r="P51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="11:17">
+      <c r="L52" t="s">
+        <v>45</v>
+      </c>
+      <c r="M52" t="s">
+        <v>55</v>
+      </c>
+      <c r="N52">
+        <v>46</v>
+      </c>
+      <c r="O52">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="11:17">
+      <c r="L53" t="s">
+        <v>19</v>
+      </c>
+      <c r="N53">
+        <v>450</v>
+      </c>
+      <c r="O53">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="11:17">
+      <c r="K54" t="s">
+        <v>30</v>
+      </c>
+      <c r="L54" t="s">
+        <v>44</v>
+      </c>
+      <c r="M54" t="s">
+        <v>56</v>
+      </c>
+      <c r="N54">
+        <v>18</v>
+      </c>
+      <c r="O54">
+        <v>4</v>
+      </c>
+      <c r="P54">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q54">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="11:17">
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <v>46</v>
+      </c>
+      <c r="O55">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="P55">
+        <v>11.1</v>
+      </c>
+      <c r="Q55">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="56" spans="11:17">
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>104</v>
+      </c>
+      <c r="O56">
+        <v>23</v>
+      </c>
+      <c r="P56">
+        <v>25.2</v>
+      </c>
+      <c r="Q56">
+        <v>40.700000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="11:17">
+      <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57">
+        <v>86</v>
+      </c>
+      <c r="O57">
+        <v>19</v>
+      </c>
+      <c r="P57">
+        <v>20.8</v>
+      </c>
+      <c r="Q57">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="58" spans="11:17">
+      <c r="M58" t="s">
+        <v>57</v>
+      </c>
+      <c r="N58">
+        <v>159</v>
+      </c>
+      <c r="O58">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="P58">
+        <v>38.5</v>
+      </c>
+      <c r="Q58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="11:17">
+      <c r="M59" t="s">
+        <v>19</v>
+      </c>
+      <c r="N59">
+        <v>413</v>
+      </c>
+      <c r="O59">
+        <v>91.4</v>
+      </c>
+      <c r="P59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="11:17">
+      <c r="L60" t="s">
+        <v>45</v>
+      </c>
+      <c r="M60" t="s">
+        <v>55</v>
+      </c>
+      <c r="N60">
+        <v>39</v>
+      </c>
+      <c r="O60">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="61" spans="11:17">
+      <c r="L61" t="s">
+        <v>19</v>
+      </c>
+      <c r="N61">
+        <v>452</v>
+      </c>
+      <c r="O61">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="11:17">
+      <c r="K62" t="s">
+        <v>32</v>
+      </c>
+      <c r="L62" t="s">
+        <v>44</v>
+      </c>
+      <c r="M62" t="s">
+        <v>56</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>0.2</v>
+      </c>
+      <c r="P62">
+        <v>0.2</v>
+      </c>
+      <c r="Q62">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="63" spans="11:17">
+      <c r="M63">
+        <v>2</v>
+      </c>
+      <c r="N63">
+        <v>24</v>
+      </c>
+      <c r="O63">
+        <v>4.8</v>
+      </c>
+      <c r="P63">
+        <v>5</v>
+      </c>
+      <c r="Q63">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="64" spans="11:17">
+      <c r="M64">
+        <v>3</v>
+      </c>
+      <c r="N64">
+        <v>60</v>
+      </c>
+      <c r="O64">
+        <v>11.9</v>
+      </c>
+      <c r="P64">
+        <v>12.5</v>
+      </c>
+      <c r="Q64">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="65" spans="12:17">
+      <c r="M65">
+        <v>4</v>
+      </c>
+      <c r="N65">
+        <v>118</v>
+      </c>
+      <c r="O65">
+        <v>23.4</v>
+      </c>
+      <c r="P65">
+        <v>24.6</v>
+      </c>
+      <c r="Q65">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="66" spans="12:17">
+      <c r="M66" t="s">
+        <v>57</v>
+      </c>
+      <c r="N66">
+        <v>277</v>
+      </c>
+      <c r="O66">
+        <v>55</v>
+      </c>
+      <c r="P66">
+        <v>57.7</v>
+      </c>
+      <c r="Q66">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="12:17">
+      <c r="M67" t="s">
+        <v>19</v>
+      </c>
+      <c r="N67">
+        <v>480</v>
+      </c>
+      <c r="O67">
+        <v>95.2</v>
+      </c>
+      <c r="P67">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="12:17">
+      <c r="L68" t="s">
+        <v>45</v>
+      </c>
+      <c r="M68" t="s">
+        <v>55</v>
+      </c>
+      <c r="N68">
+        <v>24</v>
+      </c>
+      <c r="O68">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="69" spans="12:17">
+      <c r="L69" t="s">
+        <v>19</v>
+      </c>
+      <c r="N69">
+        <v>504</v>
+      </c>
+      <c r="O69">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="17">
+    <mergeCell ref="AN3:AV3"/>
     <mergeCell ref="AD5:AE5"/>
     <mergeCell ref="AF5:AG5"/>
     <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="AJ5:AK5"/>
     <mergeCell ref="AC4:AK4"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AT4:AU4"/>
     <mergeCell ref="L4:Q4"/>
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="T6:U6"/>
@@ -5407,51 +6382,128 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E1:H4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="5:8">
-      <c r="E1" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1">
+      <c r="B1" s="1">
         <v>0.16800000000000001</v>
       </c>
-      <c r="H1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="5:8">
-      <c r="E2" t="s">
+      <c r="F1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="5:8">
-      <c r="E3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F3">
+      <c r="H2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1">
         <v>0.20599999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="5:8">
-      <c r="E4" t="s">
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F4">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>